<commit_message>
Pictures and Modified Mutations File
</commit_message>
<xml_diff>
--- a/assets/Mutations.xlsx
+++ b/assets/Mutations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Users\David B\Documents\GitHub\brunel-3\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B95595F-4237-4FF4-915B-1918A4538A00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B8940A-542F-4BF0-A850-27B638511A4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21120" windowHeight="15600" activeTab="3" xr2:uid="{17F7D696-06AE-44F4-B38F-1A100497E30D}"/>
   </bookViews>
@@ -5077,7 +5077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95096370-8A33-44C4-86A3-21EEF1D3B91C}">
   <dimension ref="A1:G184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
       <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>

</xml_diff>